<commit_message>
cleaned up db related files
</commit_message>
<xml_diff>
--- a/other/DB diagram.xlsx
+++ b/other/DB diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Web Training\3.3-Website-Login\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1134E1D7-191A-428C-A45C-2DCC5CDD08D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB036D73-C957-4287-8DFE-6DBC5C5101BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{DF2AD643-2FA4-489C-8CC6-1916DC0BF5CA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>jaarlaag</t>
   </si>
@@ -184,6 +184,33 @@
   </si>
   <si>
     <t>taak_ID</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>examennummer</t>
+  </si>
+  <si>
+    <t>adres</t>
+  </si>
+  <si>
+    <t>mobiel nummer</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>geboorte_datum</t>
+  </si>
+  <si>
+    <t>geboorte_plaats</t>
+  </si>
+  <si>
+    <t>geboorte_gemeente</t>
+  </si>
+  <si>
+    <t>geboorte_land</t>
   </si>
 </sst>
 </file>
@@ -566,27 +593,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197DF476-D301-4322-8DD4-3E86006E7737}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" customWidth="1"/>
@@ -597,71 +623,21 @@
     <col min="21" max="21" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -669,18 +645,8 @@
       <c r="C6" s="1"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="J6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -692,32 +658,8 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="J7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -725,16 +667,8 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -750,26 +684,8 @@
       <c r="E12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -778,16 +694,8 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -806,26 +714,8 @@
       <c r="F17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -841,7 +731,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -879,18 +769,206 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>